<commit_message>
pcase for LLS provider and pharmacy
</commit_message>
<xml_diff>
--- a/QA/testcases/LLS/Pharmacy/L_Phar_Patient_App_Create_PCase_Positive-OK.xlsx
+++ b/QA/testcases/LLS/Pharmacy/L_Phar_Patient_App_Create_PCase_Positive-OK.xlsx
@@ -566,10 +566,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -601,15 +601,32 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,7 +641,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,7 +664,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -647,38 +687,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -692,8 +722,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,44 +744,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -772,19 +772,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +862,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,31 +886,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,49 +898,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,19 +922,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,25 +940,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1018,6 +1018,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1040,17 +1051,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1062,6 +1062,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1089,42 +1113,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1134,127 +1134,127 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1660,10 +1660,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1831,547 +1831,563 @@
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="11"/>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9">
-        <v>3</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="B9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="11"/>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9">
-        <v>3</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="B11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="11"/>
+      <c r="B12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="9">
-        <v>3</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="11"/>
+      <c r="B14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="9">
+        <v>3</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="11"/>
+      <c r="D16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="D17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="11"/>
+      <c r="D18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="9">
-        <v>200</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="D19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="11"/>
+      <c r="D20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="9">
+        <v>200</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="9">
-        <v>3</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="12">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="B22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="9">
+        <v>3</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="9"/>
+      <c r="B23" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="11"/>
+      <c r="D24" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="9">
-        <v>2</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="12">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="B26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="D27" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="D28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="9">
-        <v>10</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="B29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="11"/>
+      <c r="B30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="9">
+        <v>15</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="9">
-        <v>10</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="B31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="11"/>
+      <c r="B32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="9">
+        <v>10</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="9" t="s">
+      <c r="B33" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="H33" s="9"/>
+      <c r="D33" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="12">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="11"/>
+      <c r="D34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="12">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9">
         <v>4</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3 B4 B7 B34:B35 C2:C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3 B4 B7 B35:B36 C2:C3">
       <formula1/>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
@@ -2380,7 +2396,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 B5:B6">
       <formula1>[3]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B11 B12:B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B9:B12 B13:B34">
       <formula1>[2]DataList!#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>